<commit_message>
Debug. Num scenarios updated.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74989CDF-5F93-4CBB-9D16-D7D2A69BE19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE128E2D-4182-4444-8BDD-85191508776B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="3696" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -1322,7 +1322,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Market data. Num scenarios increased.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D32BC1-D04B-428C-8569-6C18787BE73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B7EC71-54AE-4FC7-A81C-9B86A81050BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="3696" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1284" yWindow="1560" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Market. Num scenarios adjusted.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D32BC1-D04B-428C-8569-6C18787BE73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BE1649-F43C-4E78-A4DA-872C4F0F653A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="3696" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Market. Num scenarios increased.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BE1649-F43C-4E78-A4DA-872C4F0F653A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2545BD7B-EBBD-40B6-9CE0-972C3C75AAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Debug. Num years reduced.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2545BD7B-EBBD-40B6-9CE0-972C3C75AAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66D58F6-4690-466A-B0F8-E2C714C8FA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Debug. Market. Num scenarios updated.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66D58F6-4690-466A-B0F8-E2C714C8FA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A017B316-9507-4F7C-B9B1-DA0F5C6FDA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. Num market scenarios updated.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B71480C-B446-4FDD-B69F-4FF26F18AEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B6BD4D-4C20-463C-BF84-F8143FB134E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. 5 years, full DN
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A634A274-F2B4-4B21-9C3D-B8C88FC1C449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8F573A-8425-4A97-B67E-5E1FFA35A0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1322,7 +1322,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
Test. 5 years, DN full scns.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2025.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59022D60-DB4D-402C-97CF-9BEE5BF3A768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBD274A-7229-4FDB-8D5E-263D659ECCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>